<commit_message>
Actualizacion Planos- Sim 2
</commit_message>
<xml_diff>
--- a/XING_MAT32001 - Lista de materiales/XING_MAT32001_A2.xlsx
+++ b/XING_MAT32001 - Lista de materiales/XING_MAT32001_A2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884E1D89-0530-4D2A-B137-D526DA4324C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6414DB-58D4-415A-9530-465BF71460CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="672" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materiales SIEMENS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="165">
   <si>
     <t>Material</t>
   </si>
@@ -506,6 +506,15 @@
   </si>
   <si>
     <t xml:space="preserve">Carcazas para Fichas de conexión DB15 Salida </t>
+  </si>
+  <si>
+    <t>Cable multipolar blindado 19x0.35mm2</t>
+  </si>
+  <si>
+    <t>Cable m 19x0.35</t>
+  </si>
+  <si>
+    <t>EC 1503 [m]</t>
   </si>
 </sst>
 </file>
@@ -622,7 +631,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -725,10 +734,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -1074,9 +1086,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,7 +1333,7 @@
         <f t="shared" si="0"/>
         <v>80.8</v>
       </c>
-      <c r="F13" s="47"/>
+      <c r="F13" s="46"/>
     </row>
     <row r="14" spans="1:6" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
@@ -1478,11 +1490,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,7 +1575,7 @@
         <v>1.6659999999999999</v>
       </c>
       <c r="G3" s="20">
-        <f t="shared" ref="G3:G29" si="0">F3*E3</f>
+        <f t="shared" ref="G3:G30" si="0">F3*E3</f>
         <v>13.327999999999999</v>
       </c>
     </row>
@@ -1721,14 +1733,14 @@
         <v>4</v>
       </c>
       <c r="E10" s="40">
-        <v>380</v>
+        <v>420</v>
       </c>
       <c r="F10" s="20">
         <v>0.44600000000000001</v>
       </c>
       <c r="G10" s="20">
         <f t="shared" si="0"/>
-        <v>169.48</v>
+        <v>187.32</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -2029,7 +2041,7 @@
         <v>135</v>
       </c>
       <c r="E23" s="40">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="20">
@@ -2039,140 +2051,153 @@
     </row>
     <row r="24" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="40">
-        <v>1</v>
-      </c>
-      <c r="F24" s="20">
-        <v>1.1100000000000001</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="47">
+        <v>1.5</v>
+      </c>
+      <c r="F24" s="13"/>
       <c r="G24" s="20">
         <f t="shared" si="0"/>
-        <v>1.1100000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>5</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="40">
-        <v>600</v>
+        <v>1</v>
       </c>
       <c r="F25" s="20">
-        <v>0.01</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="G25" s="20">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="40">
-        <v>100</v>
+        <v>600</v>
       </c>
       <c r="F26" s="20">
-        <v>1.4E-2</v>
+        <v>0.01</v>
       </c>
       <c r="G26" s="20">
         <f t="shared" si="0"/>
-        <v>1.4000000000000001</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>121</v>
+        <v>15</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="D27" s="12"/>
+        <v>130</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="E27" s="40">
-        <v>2</v>
-      </c>
-      <c r="F27" s="20"/>
+        <v>100</v>
+      </c>
+      <c r="F27" s="20">
+        <v>1.4E-2</v>
+      </c>
       <c r="G27" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.4000000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>73</v>
+        <v>154</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" s="23"/>
+        <v>121</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>131</v>
+      </c>
       <c r="D28" s="12"/>
       <c r="E28" s="40">
-        <v>1</v>
-      </c>
-      <c r="F28" s="20">
-        <v>166.58</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F28" s="20"/>
       <c r="G28" s="20">
         <f t="shared" si="0"/>
-        <v>166.58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="12"/>
+        <v>74</v>
+      </c>
+      <c r="C29" s="23"/>
       <c r="D29" s="12"/>
       <c r="E29" s="40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" s="20">
-        <v>162</v>
+        <v>166.58</v>
       </c>
       <c r="G29" s="20">
         <f t="shared" si="0"/>
-        <v>324</v>
+        <v>166.58</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
+      <c r="A30" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>72</v>
+      </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
+      <c r="E30" s="40">
+        <v>2</v>
+      </c>
+      <c r="F30" s="20">
+        <v>162</v>
+      </c>
+      <c r="G30" s="20">
+        <f t="shared" si="0"/>
+        <v>324</v>
+      </c>
     </row>
     <row r="31" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
@@ -2180,7 +2205,7 @@
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="40"/>
-      <c r="F31" s="13"/>
+      <c r="F31" s="20"/>
       <c r="G31" s="20"/>
     </row>
     <row r="32" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -2189,83 +2214,83 @@
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="40"/>
-      <c r="F32" s="20"/>
+      <c r="F32" s="13"/>
       <c r="G32" s="20"/>
     </row>
     <row r="33" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>159</v>
-      </c>
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="12"/>
-      <c r="D33" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E33" s="40">
-        <v>6</v>
-      </c>
-      <c r="F33" s="13"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="20"/>
       <c r="G33" s="20"/>
     </row>
     <row r="34" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="12" t="s">
         <v>158</v>
       </c>
       <c r="E34" s="40">
-        <v>10</v>
-      </c>
-      <c r="F34" s="20"/>
+        <v>6</v>
+      </c>
+      <c r="F34" s="13"/>
       <c r="G34" s="20"/>
     </row>
     <row r="35" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C35" s="12"/>
       <c r="D35" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="E35" s="45">
-        <v>6</v>
+      <c r="E35" s="40">
+        <v>10</v>
       </c>
       <c r="F35" s="20"/>
       <c r="G35" s="20"/>
     </row>
     <row r="36" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="12" t="s">
         <v>158</v>
       </c>
       <c r="E36" s="45">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F36" s="20"/>
       <c r="G36" s="20"/>
     </row>
     <row r="37" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
+      <c r="A37" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>161</v>
+      </c>
       <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="24"/>
+      <c r="D37" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E37" s="45">
+        <v>10</v>
+      </c>
       <c r="F37" s="20"/>
       <c r="G37" s="20"/>
     </row>
@@ -2337,13 +2362,13 @@
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
-      <c r="E45" s="40"/>
+      <c r="E45" s="24"/>
       <c r="F45" s="20"/>
       <c r="G45" s="20"/>
     </row>
     <row r="46" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="38"/>
-      <c r="B46" s="38"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="40"/>
@@ -2351,8 +2376,8 @@
       <c r="G46" s="20"/>
     </row>
     <row r="47" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
+      <c r="A47" s="38"/>
+      <c r="B47" s="38"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="40"/>
@@ -2364,16 +2389,16 @@
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
-      <c r="E48" s="24"/>
+      <c r="E48" s="40"/>
       <c r="F48" s="20"/>
       <c r="G48" s="20"/>
     </row>
     <row r="49" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
-      <c r="B49" s="22"/>
+      <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
-      <c r="E49" s="40"/>
+      <c r="E49" s="24"/>
       <c r="F49" s="20"/>
       <c r="G49" s="20"/>
     </row>
@@ -2422,16 +2447,16 @@
       <c r="F54" s="20"/>
       <c r="G54" s="20"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
+      <c r="B55" s="22"/>
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
       <c r="E55" s="40"/>
-      <c r="F55" s="13"/>
+      <c r="F55" s="20"/>
       <c r="G55" s="20"/>
     </row>
-    <row r="56" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
@@ -2460,7 +2485,7 @@
     </row>
     <row r="59" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
-      <c r="B59" s="43"/>
+      <c r="B59" s="12"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
       <c r="E59" s="40"/>
@@ -2476,7 +2501,7 @@
       <c r="F60" s="13"/>
       <c r="G60" s="20"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
       <c r="B61" s="43"/>
       <c r="C61" s="12"/>
@@ -2494,9 +2519,9 @@
       <c r="F62" s="13"/>
       <c r="G62" s="20"/>
     </row>
-    <row r="63" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
+      <c r="B63" s="43"/>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="40"/>
@@ -2545,28 +2570,37 @@
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
       <c r="E68" s="40"/>
-      <c r="F68" s="20"/>
-      <c r="G68" s="25"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F69" s="18" t="s">
+      <c r="F68" s="13"/>
+      <c r="G68" s="20"/>
+    </row>
+    <row r="69" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="12"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="40"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="25"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F70" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G69" s="26">
-        <f>SUM(G2:G68)</f>
-        <v>3093.558</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="8"/>
-      <c r="D73" s="5"/>
+      <c r="G70" s="26">
+        <f>SUM(G2:G69)</f>
+        <v>3111.3980000000001</v>
+      </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="D74" s="5"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D76" s="5"/>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="8"/>
+      <c r="D75" s="5"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D77" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2838,7 +2872,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="48" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -2857,7 +2891,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
+      <c r="A4" s="48"/>
       <c r="B4" s="9" t="s">
         <v>34</v>
       </c>
@@ -2893,7 +2927,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="48" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -2912,7 +2946,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="9" t="s">
         <v>40</v>
       </c>
@@ -3247,8 +3281,8 @@
         <v>67</v>
       </c>
       <c r="B3" s="13">
-        <f>'Materiales para TABLEROS'!G69</f>
-        <v>3093.558</v>
+        <f>'Materiales para TABLEROS'!G70</f>
+        <v>3111.3980000000001</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -3293,7 +3327,7 @@
       </c>
       <c r="B7" s="19">
         <f>SUM(B2:B6)</f>
-        <v>25821.678000000004</v>
+        <v>25839.518000000004</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3302,7 +3336,7 @@
       </c>
       <c r="B8" s="36">
         <f>B7*Horas!E12</f>
-        <v>2065734.2400000002</v>
+        <v>2067161.4400000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualización LM y Planos
</commit_message>
<xml_diff>
--- a/XING_MAT32001 - Lista de materiales/XING_MAT32001_A2.xlsx
+++ b/XING_MAT32001 - Lista de materiales/XING_MAT32001_A2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213602FE-ADD0-4BDE-B5AB-1E16B7358CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4ADC17D-05A2-4A64-9A2F-57D9C9751863}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="672" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="165">
   <si>
     <t>Material</t>
   </si>
@@ -515,9 +515,6 @@
   </si>
   <si>
     <t>EC 1503 [m]</t>
-  </si>
-  <si>
-    <t>agregar bornes de hacia variador</t>
   </si>
 </sst>
 </file>
@@ -1495,9 +1492,9 @@
   </sheetPr>
   <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1736,14 +1733,14 @@
         <v>4</v>
       </c>
       <c r="E10" s="40">
-        <v>420</v>
+        <v>450</v>
       </c>
       <c r="F10" s="20">
         <v>0.44600000000000001</v>
       </c>
       <c r="G10" s="20">
         <f t="shared" si="0"/>
-        <v>187.32</v>
+        <v>200.70000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -1784,14 +1781,14 @@
         <v>4</v>
       </c>
       <c r="E12" s="40">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F12" s="20">
         <v>0.373</v>
       </c>
       <c r="G12" s="20">
         <f t="shared" si="0"/>
-        <v>20.887999999999998</v>
+        <v>22.38</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -1902,14 +1899,14 @@
         <v>134</v>
       </c>
       <c r="E17" s="40">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F17" s="20">
         <v>0.161</v>
       </c>
       <c r="G17" s="20">
         <f t="shared" si="0"/>
-        <v>8.0500000000000007</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -1926,14 +1923,14 @@
         <v>134</v>
       </c>
       <c r="E18" s="40">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F18" s="20">
         <v>0.161</v>
       </c>
       <c r="G18" s="20">
         <f t="shared" si="0"/>
-        <v>8.0500000000000007</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -1950,14 +1947,14 @@
         <v>134</v>
       </c>
       <c r="E19" s="40">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F19" s="20">
         <v>0.161</v>
       </c>
       <c r="G19" s="20">
         <f t="shared" si="0"/>
-        <v>16.100000000000001</v>
+        <v>8.0500000000000007</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -1974,14 +1971,14 @@
         <v>134</v>
       </c>
       <c r="E20" s="40">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F20" s="20">
         <v>0.161</v>
       </c>
       <c r="G20" s="20">
         <f t="shared" si="0"/>
-        <v>16.100000000000001</v>
+        <v>8.0500000000000007</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -1998,14 +1995,14 @@
         <v>134</v>
       </c>
       <c r="E21" s="40">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F21" s="20">
         <v>0.112</v>
       </c>
       <c r="G21" s="20">
         <f t="shared" si="0"/>
-        <v>44.800000000000004</v>
+        <v>22.400000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -2022,7 +2019,7 @@
         <v>135</v>
       </c>
       <c r="E22" s="40">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="20">
@@ -2044,7 +2041,7 @@
         <v>135</v>
       </c>
       <c r="E23" s="40">
-        <v>4.5</v>
+        <v>15</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="20">
@@ -2066,7 +2063,7 @@
         <v>135</v>
       </c>
       <c r="E24" s="47">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="20">
@@ -2108,14 +2105,14 @@
         <v>5</v>
       </c>
       <c r="E26" s="40">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="F26" s="20">
         <v>0.01</v>
       </c>
       <c r="G26" s="20">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -2154,7 +2151,7 @@
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20">
@@ -2335,9 +2332,7 @@
     </row>
     <row r="42" spans="1:7" s="2" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
-      <c r="B42" s="12" t="s">
-        <v>165</v>
-      </c>
+      <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="24"/>
@@ -2593,7 +2588,7 @@
       </c>
       <c r="G70" s="26">
         <f>SUM(G2:G69)</f>
-        <v>3111.3980000000001</v>
+        <v>3075.1099999999997</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3287,7 +3282,7 @@
       </c>
       <c r="B3" s="13">
         <f>'Materiales para TABLEROS'!G70</f>
-        <v>3111.3980000000001</v>
+        <v>3075.1099999999997</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -3332,7 +3327,7 @@
       </c>
       <c r="B7" s="19">
         <f>SUM(B2:B6)</f>
-        <v>25839.518000000004</v>
+        <v>25803.230000000003</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3341,7 +3336,7 @@
       </c>
       <c r="B8" s="36">
         <f>B7*Horas!E12</f>
-        <v>2067161.4400000004</v>
+        <v>2064258.4000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>